<commit_message>
Add swaps and ranges.
</commit_message>
<xml_diff>
--- a/pwflat.xlsx
+++ b/pwflat.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -386,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BACE49A-4FCE-4A52-AAC4-959EAE9753D1}">
   <dimension ref="B2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -421,7 +421,7 @@
       </c>
       <c r="C4">
         <f ca="1">RAND()</f>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
       <c r="E4">
         <v>0.1</v>
@@ -461,7 +461,7 @@
       </c>
       <c r="C7">
         <f ca="1">_xll.PWFLAT.CURVE(B3:B5, C3:C5)</f>
-        <v>370134640</v>
+        <v>-698298</v>
       </c>
       <c r="E7">
         <v>0.4</v>
@@ -531,7 +531,7 @@
       </c>
       <c r="F14">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.45">
@@ -540,7 +540,7 @@
       </c>
       <c r="F15">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.45">
@@ -549,7 +549,7 @@
       </c>
       <c r="F16">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.45">
@@ -558,7 +558,7 @@
       </c>
       <c r="F17">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.45">
@@ -567,7 +567,7 @@
       </c>
       <c r="F18">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="19" spans="5:6" x14ac:dyDescent="0.45">
@@ -576,7 +576,7 @@
       </c>
       <c r="F19">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="20" spans="5:6" x14ac:dyDescent="0.45">
@@ -585,7 +585,7 @@
       </c>
       <c r="F20">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.45">
@@ -594,7 +594,7 @@
       </c>
       <c r="F21">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.45">
@@ -603,7 +603,7 @@
       </c>
       <c r="F22">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.45">
@@ -612,7 +612,7 @@
       </c>
       <c r="F23">
         <f ca="1"/>
-        <v>0.44473887564471604</v>
+        <v>0.98547236273928163</v>
       </c>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.45">

</xml_diff>